<commit_message>
[박청아] Add / Fix - [UnitManager] 테이블 작업, 894da92 수정
</commit_message>
<xml_diff>
--- a/Content/TableData/ResourceUnit.xlsx
+++ b/Content/TableData/ResourceUnit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee\Documents\Unreal Projects\ProjectMS\Content\TableData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\capark2690\ProjectMS\Content\TableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F59921-FBFE-465A-B774-B9811EBCB34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18E7B14-1A20-4AFD-A402-10D21C22B313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,29 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Id</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Base_Path</t>
-  </si>
-  <si>
     <t>UnitType</t>
   </si>
   <si>
-    <t>GridPatternX</t>
-  </si>
-  <si>
-    <t>GridPatternY</t>
-  </si>
-  <si>
-    <t>UnitType</t>
+    <t xml:space="preserve">UnitType(EMS_UnitType) - 1 : BasePlayer, 2 : Item 3 : Furniture </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>1 : Customer, 2 : Staff</t>
+    <t>ChildTableDataType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ChildTableDataType(EMS_TableDataType) - 10 : ItemData 12 : Storage</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -402,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E5"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -416,17 +411,20 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B1" s="2"/>
       <c r="C1" s="3"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
@@ -435,14 +433,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -452,18 +446,31 @@
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
+        <v>-1</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
       <c r="C5">
         <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[이용섭] Add - [ChatWidget] 채팅 기능 완성
Add - [CheatManager/PlayerController] 치트 매니저 생성 및 적용.

Fixed - [ResourceUnit/Table] 유닛테이블 칼럼추가 및 데이터 추가(UnitName)
</commit_message>
<xml_diff>
--- a/Content/TableData/ResourceUnit.xlsx
+++ b/Content/TableData/ResourceUnit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\capark2690\ProjectMS\Content\TableData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee\Documents\Unreal Projects\ProjectMS\Content\TableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18E7B14-1A20-4AFD-A402-10D21C22B313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E7242C-F9F4-4FD0-97C9-952023A14E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="4290" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Id</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -43,6 +43,30 @@
   </si>
   <si>
     <t>ChildTableDataType(EMS_TableDataType) - 10 : ItemData 12 : Storage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UnitName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>int32</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FString</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰오리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>노오란오리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>푸르스름오리</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -50,7 +74,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,8 +104,15 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -93,8 +124,13 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -102,23 +138,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="20" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="나쁨" xfId="1" builtinId="27"/>
+    <cellStyle name="메모" xfId="2" builtinId="10"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -397,19 +454,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -417,15 +475,17 @@
       <c r="C1" s="3"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,48 +493,73 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>2</v>
       </c>
-      <c r="C5">
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>3</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>3</v>
       </c>
-      <c r="C6">
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>